<commit_message>
Creating the frequency steps
</commit_message>
<xml_diff>
--- a/test/test1-inC.xlsx
+++ b/test/test1-inC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\U_Proteomica\PROYECTOS\PESA_omicas\Metabolomics_WORKFLOW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metabolomics\bolflow\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1394,36 +1394,9 @@
     <t>H_C1824_2</t>
   </si>
   <si>
-    <t>H_QC1_all_01_1</t>
-  </si>
-  <si>
     <t>QC</t>
   </si>
   <si>
-    <t>H_QC1_all_02_1</t>
-  </si>
-  <si>
-    <t>H_QC1_all_03_1</t>
-  </si>
-  <si>
-    <t>H_QC1_all_04_1</t>
-  </si>
-  <si>
-    <t>H_QC1_all_05_1</t>
-  </si>
-  <si>
-    <t>H_QC1_all_06_1</t>
-  </si>
-  <si>
-    <t>H_QC1_all_07_2</t>
-  </si>
-  <si>
-    <t>H_QC1_all_08_2</t>
-  </si>
-  <si>
-    <t>H_QC1_all_09_2</t>
-  </si>
-  <si>
     <t>H_QC1_all_10_2</t>
   </si>
   <si>
@@ -1469,33 +1442,6 @@
     <t>H_QC1_all_24_4</t>
   </si>
   <si>
-    <t>H_QC2_all_01_1</t>
-  </si>
-  <si>
-    <t>H_QC2_all_02_1</t>
-  </si>
-  <si>
-    <t>H_QC2_all_03_1</t>
-  </si>
-  <si>
-    <t>H_QC2_all_04_1</t>
-  </si>
-  <si>
-    <t>H_QC2_all_05_1</t>
-  </si>
-  <si>
-    <t>H_QC2_all_06_1</t>
-  </si>
-  <si>
-    <t>H_QC2_all_07_2</t>
-  </si>
-  <si>
-    <t>H_QC2_all_08_2</t>
-  </si>
-  <si>
-    <t>H_QC2_all_09_2</t>
-  </si>
-  <si>
     <t>H_QC2_all_10_2</t>
   </si>
   <si>
@@ -1541,33 +1487,6 @@
     <t>H_QC2_all_24_4</t>
   </si>
   <si>
-    <t>H_QC3_all_01_1</t>
-  </si>
-  <si>
-    <t>H_QC3_all_02_1</t>
-  </si>
-  <si>
-    <t>H_QC3_all_03_1</t>
-  </si>
-  <si>
-    <t>H_QC3_all_04_1</t>
-  </si>
-  <si>
-    <t>H_QC3_all_05_1</t>
-  </si>
-  <si>
-    <t>H_QC3_all_06_1</t>
-  </si>
-  <si>
-    <t>H_QC3_all_07_2</t>
-  </si>
-  <si>
-    <t>H_QC3_all_08_2</t>
-  </si>
-  <si>
-    <t>H_QC3_all_09_2</t>
-  </si>
-  <si>
     <t>H_QC3_all_10_2</t>
   </si>
   <si>
@@ -1595,33 +1514,6 @@
     <t>H_QC3_all_18_3</t>
   </si>
   <si>
-    <t>H_QC4_all_01_1</t>
-  </si>
-  <si>
-    <t>H_QC4_all_02_1</t>
-  </si>
-  <si>
-    <t>H_QC4_all_03_1</t>
-  </si>
-  <si>
-    <t>H_QC4_all_04_1</t>
-  </si>
-  <si>
-    <t>H_QC4_all_05_1</t>
-  </si>
-  <si>
-    <t>H_QC4_all_06_1</t>
-  </si>
-  <si>
-    <t>H_QC4_all_07_2</t>
-  </si>
-  <si>
-    <t>H_QC4_all_08_2</t>
-  </si>
-  <si>
-    <t>H_QC4_all_09_2</t>
-  </si>
-  <si>
     <t>H_QC4_all_10_2</t>
   </si>
   <si>
@@ -1656,12 +1548,120 @@
   </si>
   <si>
     <t>Cohort Batch</t>
+  </si>
+  <si>
+    <t>H_QC4_all_1_1</t>
+  </si>
+  <si>
+    <t>H_QC4_all_2_1</t>
+  </si>
+  <si>
+    <t>H_QC4_all_3_1</t>
+  </si>
+  <si>
+    <t>H_QC4_all_4_1</t>
+  </si>
+  <si>
+    <t>H_QC4_all_5_1</t>
+  </si>
+  <si>
+    <t>H_QC4_all_6_1</t>
+  </si>
+  <si>
+    <t>H_QC4_all_7_2</t>
+  </si>
+  <si>
+    <t>H_QC4_all_8_2</t>
+  </si>
+  <si>
+    <t>H_QC4_all_9_2</t>
+  </si>
+  <si>
+    <t>H_QC3_all_1_1</t>
+  </si>
+  <si>
+    <t>H_QC3_all_2_1</t>
+  </si>
+  <si>
+    <t>H_QC3_all_3_1</t>
+  </si>
+  <si>
+    <t>H_QC3_all_4_1</t>
+  </si>
+  <si>
+    <t>H_QC3_all_5_1</t>
+  </si>
+  <si>
+    <t>H_QC3_all_6_1</t>
+  </si>
+  <si>
+    <t>H_QC3_all_7_2</t>
+  </si>
+  <si>
+    <t>H_QC3_all_8_2</t>
+  </si>
+  <si>
+    <t>H_QC3_all_9_2</t>
+  </si>
+  <si>
+    <t>H_QC1_all_1_1</t>
+  </si>
+  <si>
+    <t>H_QC1_all_2_1</t>
+  </si>
+  <si>
+    <t>H_QC1_all_3_1</t>
+  </si>
+  <si>
+    <t>H_QC1_all_4_1</t>
+  </si>
+  <si>
+    <t>H_QC1_all_5_1</t>
+  </si>
+  <si>
+    <t>H_QC1_all_6_1</t>
+  </si>
+  <si>
+    <t>H_QC1_all_7_2</t>
+  </si>
+  <si>
+    <t>H_QC1_all_8_2</t>
+  </si>
+  <si>
+    <t>H_QC1_all_9_2</t>
+  </si>
+  <si>
+    <t>H_QC2_all_1_1</t>
+  </si>
+  <si>
+    <t>H_QC2_all_2_1</t>
+  </si>
+  <si>
+    <t>H_QC2_all_3_1</t>
+  </si>
+  <si>
+    <t>H_QC2_all_4_1</t>
+  </si>
+  <si>
+    <t>H_QC2_all_5_1</t>
+  </si>
+  <si>
+    <t>H_QC2_all_6_1</t>
+  </si>
+  <si>
+    <t>H_QC2_all_7_2</t>
+  </si>
+  <si>
+    <t>H_QC2_all_8_2</t>
+  </si>
+  <si>
+    <t>H_QC2_all_9_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2177,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A507" workbookViewId="0">
+      <selection activeCell="A483" sqref="A483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2194,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>540</v>
+        <v>504</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2203,13 +2203,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>541</v>
+        <v>505</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>542</v>
+        <v>506</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -12521,13 +12521,13 @@
     </row>
     <row r="450" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A450" s="27" t="s">
+        <v>525</v>
+      </c>
+      <c r="B450" s="2">
+        <v>2</v>
+      </c>
+      <c r="C450" s="5" t="s">
         <v>455</v>
-      </c>
-      <c r="B450" s="2">
-        <v>2</v>
-      </c>
-      <c r="C450" s="5" t="s">
-        <v>456</v>
       </c>
       <c r="D450" s="7">
         <v>1</v>
@@ -12544,13 +12544,13 @@
     </row>
     <row r="451" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A451" s="27" t="s">
-        <v>457</v>
+        <v>526</v>
       </c>
       <c r="B451" s="2">
         <v>2</v>
       </c>
       <c r="C451" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D451" s="7">
         <v>8</v>
@@ -12567,13 +12567,13 @@
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A452" s="27" t="s">
-        <v>458</v>
+        <v>527</v>
       </c>
       <c r="B452" s="2">
         <v>2</v>
       </c>
       <c r="C452" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D452" s="7">
         <v>15</v>
@@ -12590,13 +12590,13 @@
     </row>
     <row r="453" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A453" s="27" t="s">
-        <v>459</v>
+        <v>528</v>
       </c>
       <c r="B453" s="2">
         <v>2</v>
       </c>
       <c r="C453" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D453" s="7">
         <v>22</v>
@@ -12613,13 +12613,13 @@
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" s="27" t="s">
-        <v>460</v>
+        <v>529</v>
       </c>
       <c r="B454" s="2">
         <v>2</v>
       </c>
       <c r="C454" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D454" s="7">
         <v>29</v>
@@ -12636,13 +12636,13 @@
     </row>
     <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455" s="27" t="s">
-        <v>461</v>
+        <v>530</v>
       </c>
       <c r="B455" s="2">
         <v>2</v>
       </c>
       <c r="C455" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D455" s="7">
         <v>34</v>
@@ -12659,13 +12659,13 @@
     </row>
     <row r="456" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A456" s="27" t="s">
-        <v>462</v>
+        <v>531</v>
       </c>
       <c r="B456" s="2">
         <v>2</v>
       </c>
       <c r="C456" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D456" s="7">
         <v>35</v>
@@ -12682,13 +12682,13 @@
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="27" t="s">
-        <v>463</v>
+        <v>532</v>
       </c>
       <c r="B457" s="2">
         <v>2</v>
       </c>
       <c r="C457" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D457" s="7">
         <v>42</v>
@@ -12705,13 +12705,13 @@
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" s="27" t="s">
-        <v>464</v>
+        <v>533</v>
       </c>
       <c r="B458" s="2">
         <v>2</v>
       </c>
       <c r="C458" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D458" s="7">
         <v>49</v>
@@ -12728,13 +12728,13 @@
     </row>
     <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" s="27" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="B459" s="2">
         <v>2</v>
       </c>
       <c r="C459" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D459" s="7">
         <v>56</v>
@@ -12751,13 +12751,13 @@
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="27" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="B460" s="2">
         <v>2</v>
       </c>
       <c r="C460" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D460" s="7">
         <v>63</v>
@@ -12774,13 +12774,13 @@
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A461" s="27" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="B461" s="2">
         <v>2</v>
       </c>
       <c r="C461" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D461" s="7">
         <v>72</v>
@@ -12797,13 +12797,13 @@
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" s="27" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="B462" s="2">
         <v>2</v>
       </c>
       <c r="C462" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D462" s="7">
         <v>73</v>
@@ -12820,13 +12820,13 @@
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="27" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="B463" s="2">
         <v>2</v>
       </c>
       <c r="C463" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D463" s="7">
         <v>80</v>
@@ -12843,13 +12843,13 @@
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A464" s="27" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="B464" s="2">
         <v>2</v>
       </c>
       <c r="C464" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D464" s="7">
         <v>87</v>
@@ -12866,13 +12866,13 @@
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A465" s="27" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="B465" s="2">
         <v>2</v>
       </c>
       <c r="C465" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D465" s="7">
         <v>94</v>
@@ -12889,13 +12889,13 @@
     </row>
     <row r="466" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A466" s="27" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="B466" s="2">
         <v>2</v>
       </c>
       <c r="C466" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D466" s="7">
         <v>101</v>
@@ -12912,13 +12912,13 @@
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A467" s="27" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="B467" s="2">
         <v>2</v>
       </c>
       <c r="C467" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D467" s="7">
         <v>106</v>
@@ -12935,13 +12935,13 @@
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A468" s="27" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="B468" s="2">
         <v>2</v>
       </c>
       <c r="C468" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D468" s="7">
         <v>107</v>
@@ -12958,13 +12958,13 @@
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A469" s="27" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="B469" s="2">
         <v>2</v>
       </c>
       <c r="C469" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D469" s="7">
         <v>114</v>
@@ -12981,13 +12981,13 @@
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A470" s="27" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="B470" s="2">
         <v>2</v>
       </c>
       <c r="C470" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D470" s="7">
         <v>123</v>
@@ -13004,13 +13004,13 @@
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A471" s="27" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="B471" s="2">
         <v>2</v>
       </c>
       <c r="C471" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D471" s="7">
         <v>130</v>
@@ -13027,13 +13027,13 @@
     </row>
     <row r="472" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A472" s="27" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="B472" s="2">
         <v>2</v>
       </c>
       <c r="C472" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D472" s="7">
         <v>137</v>
@@ -13050,13 +13050,13 @@
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A473" s="27" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="B473" s="2">
         <v>2</v>
       </c>
       <c r="C473" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D473" s="7">
         <v>144</v>
@@ -13073,13 +13073,13 @@
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A474" s="27" t="s">
-        <v>480</v>
+        <v>534</v>
       </c>
       <c r="B474" s="2">
         <v>3</v>
       </c>
       <c r="C474" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D474" s="12">
         <v>1</v>
@@ -13096,13 +13096,13 @@
     </row>
     <row r="475" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A475" s="27" t="s">
-        <v>481</v>
+        <v>535</v>
       </c>
       <c r="B475" s="2">
         <v>3</v>
       </c>
       <c r="C475" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D475" s="12">
         <v>8</v>
@@ -13119,13 +13119,13 @@
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A476" s="27" t="s">
-        <v>482</v>
+        <v>536</v>
       </c>
       <c r="B476" s="2">
         <v>3</v>
       </c>
       <c r="C476" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D476" s="12">
         <v>15</v>
@@ -13142,13 +13142,13 @@
     </row>
     <row r="477" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A477" s="27" t="s">
-        <v>483</v>
+        <v>537</v>
       </c>
       <c r="B477" s="2">
         <v>3</v>
       </c>
       <c r="C477" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D477" s="12">
         <v>22</v>
@@ -13165,13 +13165,13 @@
     </row>
     <row r="478" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A478" s="27" t="s">
-        <v>484</v>
+        <v>538</v>
       </c>
       <c r="B478" s="2">
         <v>3</v>
       </c>
       <c r="C478" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D478" s="12">
         <v>29</v>
@@ -13188,13 +13188,13 @@
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A479" s="27" t="s">
-        <v>485</v>
+        <v>539</v>
       </c>
       <c r="B479" s="2">
         <v>3</v>
       </c>
       <c r="C479" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D479" s="12">
         <v>34</v>
@@ -13211,13 +13211,13 @@
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A480" s="27" t="s">
-        <v>486</v>
+        <v>540</v>
       </c>
       <c r="B480" s="2">
         <v>3</v>
       </c>
       <c r="C480" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D480" s="12">
         <v>35</v>
@@ -13234,13 +13234,13 @@
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A481" s="27" t="s">
-        <v>487</v>
+        <v>541</v>
       </c>
       <c r="B481" s="2">
         <v>3</v>
       </c>
       <c r="C481" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D481" s="12">
         <v>42</v>
@@ -13257,13 +13257,13 @@
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A482" s="27" t="s">
-        <v>488</v>
+        <v>542</v>
       </c>
       <c r="B482" s="2">
         <v>3</v>
       </c>
       <c r="C482" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D482" s="12">
         <v>49</v>
@@ -13280,13 +13280,13 @@
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A483" s="27" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="B483" s="2">
         <v>3</v>
       </c>
       <c r="C483" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D483" s="12">
         <v>56</v>
@@ -13303,13 +13303,13 @@
     </row>
     <row r="484" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A484" s="27" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="B484" s="2">
         <v>3</v>
       </c>
       <c r="C484" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D484" s="12">
         <v>63</v>
@@ -13326,13 +13326,13 @@
     </row>
     <row r="485" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A485" s="27" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="B485" s="2">
         <v>3</v>
       </c>
       <c r="C485" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D485" s="12">
         <v>72</v>
@@ -13349,13 +13349,13 @@
     </row>
     <row r="486" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A486" s="27" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="B486" s="2">
         <v>3</v>
       </c>
       <c r="C486" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D486" s="12">
         <v>73</v>
@@ -13372,13 +13372,13 @@
     </row>
     <row r="487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A487" s="27" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="B487" s="2">
         <v>3</v>
       </c>
       <c r="C487" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D487" s="12">
         <v>80</v>
@@ -13395,13 +13395,13 @@
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" s="27" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="B488" s="2">
         <v>3</v>
       </c>
       <c r="C488" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D488" s="12">
         <v>87</v>
@@ -13418,13 +13418,13 @@
     </row>
     <row r="489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A489" s="27" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="B489" s="2">
         <v>3</v>
       </c>
       <c r="C489" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D489" s="12">
         <v>94</v>
@@ -13441,13 +13441,13 @@
     </row>
     <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490" s="27" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B490" s="2">
         <v>3</v>
       </c>
       <c r="C490" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D490" s="12">
         <v>101</v>
@@ -13464,13 +13464,13 @@
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A491" s="27" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="B491" s="2">
         <v>3</v>
       </c>
       <c r="C491" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D491" s="12">
         <v>106</v>
@@ -13487,13 +13487,13 @@
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A492" s="27" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="B492" s="2">
         <v>3</v>
       </c>
       <c r="C492" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D492" s="12">
         <v>107</v>
@@ -13510,13 +13510,13 @@
     </row>
     <row r="493" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A493" s="27" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="B493" s="2">
         <v>3</v>
       </c>
       <c r="C493" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D493" s="12">
         <v>114</v>
@@ -13533,13 +13533,13 @@
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A494" s="27" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="B494" s="2">
         <v>3</v>
       </c>
       <c r="C494" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D494" s="12">
         <v>123</v>
@@ -13556,13 +13556,13 @@
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A495" s="27" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="B495" s="2">
         <v>3</v>
       </c>
       <c r="C495" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D495" s="12">
         <v>130</v>
@@ -13579,13 +13579,13 @@
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A496" s="27" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="B496" s="2">
         <v>3</v>
       </c>
       <c r="C496" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D496" s="12">
         <v>137</v>
@@ -13602,13 +13602,13 @@
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A497" s="27" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="B497" s="2">
         <v>3</v>
       </c>
       <c r="C497" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D497" s="12">
         <v>144</v>
@@ -13625,13 +13625,13 @@
     </row>
     <row r="498" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A498" s="27" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="B498" s="2">
         <v>4</v>
       </c>
       <c r="C498" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D498" s="15">
         <v>1</v>
@@ -13648,13 +13648,13 @@
     </row>
     <row r="499" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A499" s="27" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="B499" s="2">
         <v>4</v>
       </c>
       <c r="C499" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D499" s="15">
         <v>8</v>
@@ -13671,13 +13671,13 @@
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A500" s="27" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="B500" s="2">
         <v>4</v>
       </c>
       <c r="C500" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D500" s="15">
         <v>15</v>
@@ -13694,13 +13694,13 @@
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A501" s="27" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B501" s="2">
         <v>4</v>
       </c>
       <c r="C501" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D501" s="15">
         <v>22</v>
@@ -13717,13 +13717,13 @@
     </row>
     <row r="502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A502" s="27" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="B502" s="2">
         <v>4</v>
       </c>
       <c r="C502" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D502" s="15">
         <v>31</v>
@@ -13740,13 +13740,13 @@
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A503" s="27" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="B503" s="2">
         <v>4</v>
       </c>
       <c r="C503" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D503" s="15">
         <v>40</v>
@@ -13763,13 +13763,13 @@
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A504" s="27" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
       <c r="B504" s="2">
         <v>4</v>
       </c>
       <c r="C504" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D504" s="15">
         <v>41</v>
@@ -13786,13 +13786,13 @@
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A505" s="27" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="B505" s="2">
         <v>4</v>
       </c>
       <c r="C505" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D505" s="15">
         <v>48</v>
@@ -13809,13 +13809,13 @@
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" s="27" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="B506" s="2">
         <v>4</v>
       </c>
       <c r="C506" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D506" s="15">
         <v>55</v>
@@ -13832,13 +13832,13 @@
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A507" s="27" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="B507" s="2">
         <v>4</v>
       </c>
       <c r="C507" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D507" s="15">
         <v>62</v>
@@ -13855,13 +13855,13 @@
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A508" s="27" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="B508" s="2">
         <v>4</v>
       </c>
       <c r="C508" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D508" s="15">
         <v>71</v>
@@ -13878,13 +13878,13 @@
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A509" s="27" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="B509" s="2">
         <v>4</v>
       </c>
       <c r="C509" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D509" s="15">
         <v>80</v>
@@ -13901,13 +13901,13 @@
     </row>
     <row r="510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A510" s="27" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="B510" s="2">
         <v>4</v>
       </c>
       <c r="C510" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D510" s="15">
         <v>81</v>
@@ -13924,13 +13924,13 @@
     </row>
     <row r="511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A511" s="27" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="B511" s="2">
         <v>4</v>
       </c>
       <c r="C511" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D511" s="15">
         <v>88</v>
@@ -13947,13 +13947,13 @@
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A512" s="27" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
       <c r="B512" s="2">
         <v>4</v>
       </c>
       <c r="C512" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D512" s="15">
         <v>95</v>
@@ -13970,13 +13970,13 @@
     </row>
     <row r="513" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A513" s="27" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="B513" s="2">
         <v>4</v>
       </c>
       <c r="C513" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D513" s="15">
         <v>102</v>
@@ -13993,13 +13993,13 @@
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A514" s="27" t="s">
-        <v>520</v>
+        <v>493</v>
       </c>
       <c r="B514" s="2">
         <v>4</v>
       </c>
       <c r="C514" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D514" s="15">
         <v>111</v>
@@ -14016,13 +14016,13 @@
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A515" s="27" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
       <c r="B515" s="2">
         <v>4</v>
       </c>
       <c r="C515" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D515" s="15">
         <v>120</v>
@@ -14039,13 +14039,13 @@
     </row>
     <row r="516" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A516" s="27" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="B516" s="2">
         <v>5</v>
       </c>
       <c r="C516" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D516" s="1">
         <v>1</v>
@@ -14062,13 +14062,13 @@
     </row>
     <row r="517" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A517" s="27" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="B517" s="2">
         <v>5</v>
       </c>
       <c r="C517" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D517" s="1">
         <v>8</v>
@@ -14085,13 +14085,13 @@
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A518" s="27" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
       <c r="B518" s="2">
         <v>5</v>
       </c>
       <c r="C518" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D518" s="1">
         <v>15</v>
@@ -14108,13 +14108,13 @@
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A519" s="27" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="B519" s="2">
         <v>5</v>
       </c>
       <c r="C519" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D519" s="1">
         <v>22</v>
@@ -14131,13 +14131,13 @@
     </row>
     <row r="520" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A520" s="27" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="B520" s="2">
         <v>5</v>
       </c>
       <c r="C520" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D520" s="1">
         <v>31</v>
@@ -14154,13 +14154,13 @@
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A521" s="27" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="B521" s="2">
         <v>5</v>
       </c>
       <c r="C521" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D521" s="1">
         <v>40</v>
@@ -14177,13 +14177,13 @@
     </row>
     <row r="522" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A522" s="27" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="B522" s="2">
         <v>5</v>
       </c>
       <c r="C522" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D522" s="1">
         <v>41</v>
@@ -14200,13 +14200,13 @@
     </row>
     <row r="523" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A523" s="27" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="B523" s="2">
         <v>5</v>
       </c>
       <c r="C523" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D523" s="1">
         <v>48</v>
@@ -14223,13 +14223,13 @@
     </row>
     <row r="524" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A524" s="27" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="B524" s="2">
         <v>5</v>
       </c>
       <c r="C524" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D524" s="1">
         <v>55</v>
@@ -14246,13 +14246,13 @@
     </row>
     <row r="525" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A525" s="27" t="s">
-        <v>531</v>
+        <v>495</v>
       </c>
       <c r="B525" s="2">
         <v>5</v>
       </c>
       <c r="C525" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D525" s="1">
         <v>62</v>
@@ -14269,13 +14269,13 @@
     </row>
     <row r="526" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A526" s="27" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="B526" s="2">
         <v>5</v>
       </c>
       <c r="C526" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D526" s="1">
         <v>71</v>
@@ -14292,13 +14292,13 @@
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A527" s="27" t="s">
-        <v>533</v>
+        <v>497</v>
       </c>
       <c r="B527" s="2">
         <v>5</v>
       </c>
       <c r="C527" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D527" s="1">
         <v>80</v>
@@ -14315,13 +14315,13 @@
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A528" s="27" t="s">
-        <v>534</v>
+        <v>498</v>
       </c>
       <c r="B528" s="2">
         <v>5</v>
       </c>
       <c r="C528" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D528" s="1">
         <v>81</v>
@@ -14338,13 +14338,13 @@
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A529" s="27" t="s">
-        <v>535</v>
+        <v>499</v>
       </c>
       <c r="B529" s="2">
         <v>5</v>
       </c>
       <c r="C529" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D529" s="1">
         <v>88</v>
@@ -14361,13 +14361,13 @@
     </row>
     <row r="530" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A530" s="27" t="s">
-        <v>536</v>
+        <v>500</v>
       </c>
       <c r="B530" s="2">
         <v>5</v>
       </c>
       <c r="C530" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D530" s="1">
         <v>95</v>
@@ -14384,13 +14384,13 @@
     </row>
     <row r="531" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A531" s="27" t="s">
-        <v>537</v>
+        <v>501</v>
       </c>
       <c r="B531" s="2">
         <v>5</v>
       </c>
       <c r="C531" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D531" s="1">
         <v>102</v>
@@ -14407,13 +14407,13 @@
     </row>
     <row r="532" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A532" s="27" t="s">
-        <v>538</v>
+        <v>502</v>
       </c>
       <c r="B532" s="2">
         <v>5</v>
       </c>
       <c r="C532" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D532" s="1">
         <v>111</v>
@@ -14430,13 +14430,13 @@
     </row>
     <row r="533" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A533" s="27" t="s">
-        <v>539</v>
+        <v>503</v>
       </c>
       <c r="B533" s="2">
         <v>5</v>
       </c>
       <c r="C533" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D533" s="1">
         <v>120</v>

</xml_diff>